<commit_message>
updated zeitplan and projectjournal
</commit_message>
<xml_diff>
--- a/documentation/arbeitsplan.xlsx
+++ b/documentation/arbeitsplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias.Tonini\Documents\GitHub\tnt\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias.Tonini\Documents\git\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1033,17 +1033,23 @@
         <f t="shared" ref="F9:F25" si="1">MROUND(E9*1.2*1.1,0.5)</f>
         <v>5.5</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="str">
+      <c r="G9" s="7">
+        <v>4</v>
+      </c>
+      <c r="H9" s="7">
         <f>IF(G9="","",SUM($F$7:F9)-SUM($G$7:G9))</f>
-        <v/>
+        <v>5.5</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="J9" s="14">
+        <v>43415</v>
+      </c>
+      <c r="K9" s="14">
+        <v>43473</v>
+      </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
@@ -1060,17 +1066,23 @@
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7" t="str">
+      <c r="G10" s="7">
+        <v>4</v>
+      </c>
+      <c r="H10" s="7">
         <f>IF(G10="","",SUM($F$7:F10)-SUM($G$7:G10))</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="J10" s="14">
+        <v>43415</v>
+      </c>
+      <c r="K10" s="14">
+        <v>43473</v>
+      </c>
     </row>
     <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
@@ -1087,17 +1099,23 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7" t="str">
+      <c r="G11" s="7">
+        <v>5.5</v>
+      </c>
+      <c r="H11" s="7">
         <f>IF(G11="","",SUM($F$7:F11)-SUM($G$7:G11))</f>
-        <v/>
+        <v>9.5</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="14">
+        <v>43415</v>
+      </c>
+      <c r="K11" s="14">
+        <v>43473</v>
+      </c>
     </row>
     <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
@@ -1114,17 +1132,23 @@
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7" t="str">
+      <c r="G12" s="7">
+        <v>7</v>
+      </c>
+      <c r="H12" s="7">
         <f>IF(G12="","",SUM($F$7:F12)-SUM($G$7:G12))</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="J12" s="14">
+        <v>43415</v>
+      </c>
+      <c r="K12" s="14">
+        <v>43473</v>
+      </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="22"/>
@@ -1141,17 +1165,23 @@
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="str">
+      <c r="G13" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="7">
         <f>IF(G13="","",SUM($F$7:F13)-SUM($G$7:G13))</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="J13" s="14">
+        <v>43415</v>
+      </c>
+      <c r="K13" s="14">
+        <v>43473</v>
+      </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
@@ -1170,17 +1200,23 @@
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="str">
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7">
         <f>IF(G14="","",SUM($F$7:F14)-SUM($G$7:G14))</f>
-        <v/>
+        <v>9.5</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="14">
+        <v>43480</v>
+      </c>
+      <c r="K14" s="14">
+        <v>43480</v>
+      </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B15" s="25"/>
@@ -1197,17 +1233,23 @@
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="str">
+      <c r="G15" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="H15" s="7">
         <f>IF(G15="","",SUM($F$7:F15)-SUM($G$7:G15))</f>
-        <v/>
+        <v>10.5</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="J15" s="14">
+        <v>43515</v>
+      </c>
+      <c r="K15" s="14">
+        <v>43550</v>
+      </c>
     </row>
     <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B16" s="25"/>
@@ -1224,14 +1266,23 @@
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="7">
+        <v>10.5</v>
+      </c>
+      <c r="H16" s="7">
+        <f>IF(G16="","",SUM($F$7:F16)-SUM($G$7:G16))</f>
+        <v>10.5</v>
+      </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
+      <c r="J16" s="14">
+        <v>43515</v>
+      </c>
+      <c r="K16" s="14">
+        <v>43529</v>
+      </c>
     </row>
     <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B17" s="25"/>
@@ -1249,13 +1300,18 @@
         <v>5.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="str">
+        <f>IF(G17="","",SUM($F$7:F17)-SUM($G$7:G17))</f>
+        <v/>
+      </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="J17" s="14">
+        <v>43522</v>
+      </c>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B18" s="25"/>
@@ -1273,7 +1329,10 @@
         <v>8</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="str">
+        <f>IF(G18="","",SUM($F$7:F18)-SUM($G$7:G18))</f>
+        <v/>
+      </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
@@ -1297,7 +1356,10 @@
         <v>8</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="str">
+        <f>IF(G19="","",SUM($F$7:F19)-SUM($G$7:G19))</f>
+        <v/>
+      </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
@@ -1321,7 +1383,10 @@
         <v>8</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="7" t="str">
+        <f>IF(G20="","",SUM($F$7:F20)-SUM($G$7:G20))</f>
+        <v/>
+      </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
@@ -1490,7 +1555,7 @@
       </c>
       <c r="G27" s="9">
         <f>SUM(G7:G26)</f>
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="12">

</xml_diff>